<commit_message>
V1.3.1_RELEASE is finished -- all has been done1
</commit_message>
<xml_diff>
--- a/results/Visualize.xlsx
+++ b/results/Visualize.xlsx
@@ -12,9 +12,6 @@
   <definedNames>
     <definedName name="_xlchart.v3.0" hidden="1">Sheet1!$M$20:$N$25</definedName>
     <definedName name="_xlchart.v3.1" hidden="1">Sheet1!$O$20:$O$25</definedName>
-    <definedName name="_xlchart.v3.2" hidden="1">Sheet1!$O$20:$O$25</definedName>
-    <definedName name="_xlchart.v3.3" hidden="1">Sheet1!$M$20:$N$25</definedName>
-    <definedName name="_xlchart.v3.4" hidden="1">Sheet1!$O$20:$O$25</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
   <si>
     <t>广东</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -101,10 +98,6 @@
   </si>
   <si>
     <t>婚姻状态分析</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>地区平均年龄分析</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -188,6 +181,102 @@
   </si>
   <si>
     <t>女性地区平均身高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>湖北</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地区平均年龄分析(男)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>广东</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上海</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>湖南</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>浙江</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重庆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>云南</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北京</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陕西</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>江苏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天津</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吉林</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>四川</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>安徽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地区平均年龄分析(女)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>湖南</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陕西</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北京</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>浙江</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>云南</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重庆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>四川</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>湖北</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -695,7 +784,6 @@
               <a:rPr lang="zh-CN" altLang="en-US"/>
               <a:t>婚姻状态分析</a:t>
             </a:r>
-            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -750,6 +838,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-DC64-4546-8BC6-4A25B2A50564}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -765,6 +858,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-DC64-4546-8BC6-4A25B2A50564}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -780,6 +878,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-DC64-4546-8BC6-4A25B2A50564}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -969,367 +1072,6 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US"/>
-              <a:t>地区平均年龄分析</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$20:$A$33</c:f>
-              <c:strCache>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>安徽</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>四川</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>天津</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>吉林</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>江苏</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>重庆</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>云南</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>浙江</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>湖北</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>广东</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>陕西</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>北京</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>湖南</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>上海</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$20:$B$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>25.197399999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>25.336600000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>25.379000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25.438199999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25.538799999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25.631799999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>25.717500000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>25.7776</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>25.779599999999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>25.815200000000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>25.901499999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>25.9575</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>26.1097</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>26.1691</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2440-4028-AF87-647A6FED9A02}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="751392712"/>
-        <c:axId val="751389432"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="751392712"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="751389432"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="751389432"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="751392712"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -1689,7 +1431,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -2049,15 +1791,753 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:t>平均年龄</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>-</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:t>男</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$20:$A$33</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>湖北</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>广东</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>上海</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>湖南</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>浙江</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>重庆</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>云南</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>北京</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>陕西</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>江苏</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>吉林</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>天津</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>四川</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>安徽</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$20:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>26.132899999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.083200000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.069600000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.918500000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.837900000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.826000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.7255</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25.674099999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25.517199999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25.512699999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25.380800000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25.204999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24.8538</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EEDB-43E3-86A8-C9AC830906E4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="11623664"/>
+        <c:axId val="340455504"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="11623664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="340455504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="340455504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="11623664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:t>平均年龄</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>-</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:t>女</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$56:$A$69</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>上海</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>湖南</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>陕西</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>北京</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>安徽</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>浙江</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>云南</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>江苏</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>广东</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>重庆</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>四川</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>湖北</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>天津</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>吉林</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$56:$B$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>26.264800000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.1662</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.136900000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.127400000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.656300000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.605799999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.585999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.566700000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25.5425</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25.4542</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25.451499999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25.428999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25.376999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25.369800000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9B83-4911-A167-9C71E588FEEE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="611686488"/>
+        <c:axId val="611684520"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="611686488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="611684520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="611684520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="611686488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v3.3</cx:f>
+        <cx:f>_xlchart.v3.0</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v3.4</cx:f>
+        <cx:f>_xlchart.v3.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2336,6 +2816,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3359,7 +3879,517 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="381">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3563,22 +4593,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -3683,8 +4714,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3816,19 +4847,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3857,516 +4889,6 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="381">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat">
-        <a:solidFill>
-          <a:srgbClr val="D9D9D9"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -4877,7 +5399,7 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5081,23 +5603,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -5202,8 +5723,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5335,20 +5856,522 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -5457,42 +6480,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>90487</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>547687</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="图表 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01EB419E-04C9-43AC-866F-2E77C3A30408}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>214312</xdr:colOff>
       <xdr:row>18</xdr:row>
@@ -5523,7 +6510,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -5599,7 +6586,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5635,7 +6622,79 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76E861C1-D83A-4F0B-807E-89D23B1FC5EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>461962</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDA6AB3A-09B1-4B9E-BC16-3ECD43F48395}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5941,10 +7000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="L60" sqref="L60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6091,24 +7150,24 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="B19" s="4"/>
       <c r="M19" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B20">
-        <v>25.197399999999998</v>
+        <v>26.132899999999999</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N20" s="3"/>
       <c r="O20" s="1">
@@ -6117,13 +7176,13 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="B21">
-        <v>25.336600000000001</v>
+        <v>26.083200000000001</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N21" s="3"/>
       <c r="O21" s="1">
@@ -6132,13 +7191,13 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B22">
-        <v>25.379000000000001</v>
+        <v>26.069600000000001</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N22" s="3"/>
       <c r="O22" s="1">
@@ -6147,13 +7206,13 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="B23">
-        <v>25.438199999999998</v>
+        <v>26.06</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N23" s="3"/>
       <c r="O23" s="1">
@@ -6162,13 +7221,13 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="B24">
-        <v>25.538799999999998</v>
+        <v>25.918500000000002</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N24" s="3"/>
       <c r="O24" s="1">
@@ -6177,13 +7236,13 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="B25">
-        <v>25.631799999999998</v>
+        <v>25.837900000000001</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N25" s="3"/>
       <c r="O25" s="1">
@@ -6192,75 +7251,75 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B26">
-        <v>25.717500000000001</v>
+        <v>25.826000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="B27">
-        <v>25.7776</v>
+        <v>25.7255</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="B28">
-        <v>25.779599999999999</v>
+        <v>25.674099999999999</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="B29">
-        <v>25.815200000000001</v>
+        <v>25.517199999999999</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="B30">
-        <v>25.901499999999999</v>
+        <v>25.512699999999999</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="B31">
-        <v>25.9575</v>
+        <v>25.380800000000001</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="B32">
-        <v>26.1097</v>
+        <v>25.204999999999998</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="B33">
-        <v>26.1691</v>
+        <v>24.8538</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37" s="4"/>
       <c r="M37" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N37" s="4"/>
     </row>
@@ -6272,7 +7331,7 @@
         <v>175.51249999999999</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N38" s="1">
         <v>171.92019999999999</v>
@@ -6286,7 +7345,7 @@
         <v>175.483</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N39" s="1">
         <v>164.05099999999999</v>
@@ -6294,13 +7353,13 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B40" s="1">
         <v>175.2978</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N40" s="1">
         <v>163.79519999999999</v>
@@ -6314,7 +7373,7 @@
         <v>174.95179999999999</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N41" s="1">
         <v>162.93559999999999</v>
@@ -6322,13 +7381,13 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B42" s="1">
         <v>174.80799999999999</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N42" s="1">
         <v>162.8639</v>
@@ -6336,13 +7395,13 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43" s="1">
         <v>174.16059999999999</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N43" s="1">
         <v>162.74180000000001</v>
@@ -6370,7 +7429,7 @@
         <v>173.67949999999999</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N45" s="1">
         <v>162.2063</v>
@@ -6384,7 +7443,7 @@
         <v>172.98840000000001</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N46" s="1">
         <v>161.65270000000001</v>
@@ -6398,7 +7457,7 @@
         <v>172.97929999999999</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N47" s="1">
         <v>161.5976</v>
@@ -6434,7 +7493,7 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B50" s="1">
         <v>172.02940000000001</v>
@@ -6448,7 +7507,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B51" s="1">
         <v>160.35749999999999</v>
@@ -6462,12 +7521,134 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="4"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>43</v>
+      </c>
+      <c r="B56">
+        <v>26.264800000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>26.1662</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>26.136900000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>26.127400000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>54</v>
+      </c>
+      <c r="B60">
+        <v>25.656300000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>25.605799999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>25.585999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>50</v>
+      </c>
+      <c r="B63">
+        <v>25.566700000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>42</v>
+      </c>
+      <c r="B64">
+        <v>25.5425</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>61</v>
+      </c>
+      <c r="B65">
+        <v>25.4542</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>62</v>
+      </c>
+      <c r="B66">
+        <v>25.451499999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>63</v>
+      </c>
+      <c r="B67">
+        <v>25.428999999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>51</v>
+      </c>
+      <c r="B68">
+        <v>25.376999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>52</v>
+      </c>
+      <c r="B69">
+        <v>25.369800000000001</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A20:B33">
     <sortCondition ref="B20:B33"/>
   </sortState>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A55:B55"/>
     <mergeCell ref="M24:N24"/>
     <mergeCell ref="M25:N25"/>
     <mergeCell ref="M19:O19"/>
@@ -6477,9 +7658,6 @@
     <mergeCell ref="M21:N21"/>
     <mergeCell ref="M22:N22"/>
     <mergeCell ref="M23:N23"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A19:B19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>